<commit_message>
Continued final report risk of bias
</commit_message>
<xml_diff>
--- a/input/raw_data/final_report/bias_assessment_case_series_end.xlsx
+++ b/input/raw_data/final_report/bias_assessment_case_series_end.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jackgedge/Projects/msc_dissertation/iifo_motivation/input/raw_data/final_report/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A6D203B-3C49-8C41-9085-BCF28F0B96E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F623463D-7E1E-DF40-975C-B7BDB3D2EF71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20580" yWindow="880" windowWidth="20560" windowHeight="24440" xr2:uid="{2EF234BE-2A19-EE48-AF33-412A086BBDEA}"/>
   </bookViews>
@@ -1004,7 +1004,7 @@
   <dimension ref="A1:T21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>